<commit_message>
Added RF and Boosted Tree tables
</commit_message>
<xml_diff>
--- a/AllState_VariableTable.xlsx
+++ b/AllState_VariableTable.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21360" yWindow="2060" windowWidth="20280" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="-28120" yWindow="2440" windowWidth="20280" windowHeight="16600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Variable Desc" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Variable Name</t>
   </si>
@@ -213,13 +214,67 @@
   </si>
   <si>
     <t>Interval/Ratio</t>
+  </si>
+  <si>
+    <t>A_change</t>
+  </si>
+  <si>
+    <t>B_change</t>
+  </si>
+  <si>
+    <t>C_change</t>
+  </si>
+  <si>
+    <t>D_change</t>
+  </si>
+  <si>
+    <t>E_change</t>
+  </si>
+  <si>
+    <t>F_change</t>
+  </si>
+  <si>
+    <t>G_change</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Option G</t>
+  </si>
+  <si>
+    <t>post.valid.boost.G</t>
+  </si>
+  <si>
+    <t>Class: 1</t>
+  </si>
+  <si>
+    <t>Class: 2</t>
+  </si>
+  <si>
+    <t>Class: 3</t>
+  </si>
+  <si>
+    <t>Class: 4</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Boosted Tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,16 +298,75 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -260,8 +374,280 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -271,22 +657,115 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="21">
+    <cellStyle name="Calculation" xfId="10" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -325,11 +804,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E27:F34" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E27:F34" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="E27:F34"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Option Name" dataDxfId="3"/>
-    <tableColumn id="2" name="Possible Values" dataDxfId="2"/>
+    <tableColumn id="1" name="Option Name" dataDxfId="1"/>
+    <tableColumn id="2" name="Possible Values" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -600,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,4 +1385,384 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>6894</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6392</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6716</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4927</v>
+      </c>
+      <c r="F5" s="7">
+        <v>6067</v>
+      </c>
+      <c r="G5" s="5">
+        <v>7039</v>
+      </c>
+      <c r="H5" s="4">
+        <v>13174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="H13" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="15">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="22">
+        <v>4271</v>
+      </c>
+      <c r="D15" s="4">
+        <v>729</v>
+      </c>
+      <c r="E15" s="4">
+        <v>246</v>
+      </c>
+      <c r="F15" s="17">
+        <v>60</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.8881</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.87360000000000004</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.73258000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4">
+        <v>607</v>
+      </c>
+      <c r="D16" s="22">
+        <v>8436</v>
+      </c>
+      <c r="E16" s="4">
+        <v>548</v>
+      </c>
+      <c r="F16" s="17">
+        <v>180</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.94640000000000002</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.90969999999999995</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.95820000000000005</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.98663000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>132</v>
+      </c>
+      <c r="D17" s="4">
+        <v>263</v>
+      </c>
+      <c r="E17" s="22">
+        <v>6697</v>
+      </c>
+      <c r="F17" s="17">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20">
+        <v>4</v>
+      </c>
+      <c r="C18" s="21">
+        <v>36</v>
+      </c>
+      <c r="D18" s="21">
+        <v>75</v>
+      </c>
+      <c r="E18" s="21">
+        <v>174</v>
+      </c>
+      <c r="F18" s="23">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>3</v>
+      </c>
+      <c r="F23" s="15">
+        <v>4</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0.8468</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.89170000000000005</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.87490000000000001</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0.73111000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="22">
+        <v>4273</v>
+      </c>
+      <c r="D24" s="4">
+        <v>710</v>
+      </c>
+      <c r="E24" s="4">
+        <v>252</v>
+      </c>
+      <c r="F24" s="17">
+        <v>62</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0.94669999999999999</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0.90969999999999995</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.95960000000000001</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0.98726000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>619</v>
+      </c>
+      <c r="D25" s="22">
+        <v>8474</v>
+      </c>
+      <c r="E25" s="4">
+        <v>536</v>
+      </c>
+      <c r="F25" s="17">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4">
+        <v>116</v>
+      </c>
+      <c r="D26" s="4">
+        <v>245</v>
+      </c>
+      <c r="E26" s="22">
+        <v>6706</v>
+      </c>
+      <c r="F26" s="17">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20">
+        <v>4</v>
+      </c>
+      <c r="C27" s="21">
+        <v>38</v>
+      </c>
+      <c r="D27" s="21">
+        <v>74</v>
+      </c>
+      <c r="E27" s="21">
+        <v>171</v>
+      </c>
+      <c r="F27" s="23">
+        <v>1490</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A13:B14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>